<commit_message>
student home teacher home tentative study plan
</commit_message>
<xml_diff>
--- a/data/enrollments.xlsx
+++ b/data/enrollments.xlsx
@@ -36,8 +36,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -65,8 +73,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -350,7 +359,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -359,14 +368,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated CSS for mobile responsiveness
</commit_message>
<xml_diff>
--- a/data/enrollments.xlsx
+++ b/data/enrollments.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>Roll_No</t>
   </si>
@@ -39,6 +39,12 @@
   </si>
   <si>
     <t>CL-0001</t>
+  </si>
+  <si>
+    <t>MT-0001</t>
+  </si>
+  <si>
+    <t>SS-0001</t>
   </si>
 </sst>
 </file>
@@ -365,14 +371,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -400,6 +407,22 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Student and Course list pages added for teacher
</commit_message>
<xml_diff>
--- a/data/enrollments.xlsx
+++ b/data/enrollments.xlsx
@@ -14,48 +14,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
-  <si>
-    <t>Roll_No</t>
-  </si>
-  <si>
-    <t>Course_Code</t>
-  </si>
-  <si>
-    <t>F-22-SE-A-3001</t>
-  </si>
-  <si>
-    <t>CS-0001</t>
-  </si>
-  <si>
-    <t>CL-0001</t>
-  </si>
-  <si>
-    <t>MT-0001</t>
-  </si>
-  <si>
-    <t>SS-0001</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -66,14 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -85,14 +49,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
@@ -398,57 +356,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="16.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="13.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="1" width="16.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="1" width="13.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
-  <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>